<commit_message>
also added TX_PROGDIV_CFG to slink protocol manually
</commit_message>
<xml_diff>
--- a/examples/EMTF_vu13p_r1/src/protocol_SLINK.xlsx
+++ b/examples/EMTF_vu13p_r1/src/protocol_SLINK.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="slink_mgt_atts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="1143">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -1913,6 +1913,12 @@
   </si>
   <si>
     <t xml:space="preserve">PREPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX_PROGDIV_CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.5</t>
   </si>
   <si>
     <t xml:space="preserve">TX_PROGDIV_RATE</t>
@@ -3579,10 +3585,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D717"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A448" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A479" activeCellId="0" sqref="A479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8343,17 +8349,17 @@
         <v>630</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>10</v>
+        <v>631</v>
       </c>
       <c r="C476" s="0"/>
       <c r="D476" s="0"/>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>632</v>
+        <v>10</v>
       </c>
       <c r="C477" s="0"/>
       <c r="D477" s="0"/>
@@ -8363,67 +8369,67 @@
         <v>633</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>105</v>
+        <v>634</v>
       </c>
       <c r="C478" s="0"/>
       <c r="D478" s="0"/>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>256</v>
+        <v>105</v>
       </c>
       <c r="C479" s="0"/>
       <c r="D479" s="0"/>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="C480" s="0"/>
       <c r="D480" s="0"/>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>592</v>
+        <v>115</v>
       </c>
       <c r="C481" s="0"/>
       <c r="D481" s="0"/>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>29</v>
+        <v>592</v>
       </c>
       <c r="C482" s="0"/>
       <c r="D482" s="0"/>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>472</v>
+        <v>29</v>
       </c>
       <c r="C483" s="0"/>
       <c r="D483" s="0"/>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>640</v>
+        <v>472</v>
       </c>
       <c r="C484" s="0"/>
       <c r="D484" s="0"/>
@@ -8433,17 +8439,17 @@
         <v>641</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>6</v>
+        <v>642</v>
       </c>
       <c r="C485" s="0"/>
       <c r="D485" s="0"/>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>643</v>
+        <v>6</v>
       </c>
       <c r="C486" s="0"/>
       <c r="D486" s="0"/>
@@ -8463,27 +8469,27 @@
         <v>646</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>6</v>
+        <v>647</v>
       </c>
       <c r="C488" s="0"/>
       <c r="D488" s="0"/>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C489" s="0"/>
       <c r="D489" s="0"/>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>649</v>
+        <v>29</v>
       </c>
       <c r="C490" s="0"/>
       <c r="D490" s="0"/>
@@ -8573,24 +8579,24 @@
         <v>666</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>29</v>
+        <v>667</v>
       </c>
       <c r="C499" s="0"/>
       <c r="D499" s="0"/>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C500" s="0"/>
       <c r="D500" s="0"/>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B501" s="3" t="s">
         <v>6</v>
@@ -8600,10 +8606,10 @@
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B502" s="3" t="s">
-        <v>670</v>
+        <v>6</v>
       </c>
       <c r="C502" s="0"/>
       <c r="D502" s="0"/>
@@ -8633,34 +8639,34 @@
         <v>675</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>189</v>
+        <v>676</v>
       </c>
       <c r="C505" s="0"/>
       <c r="D505" s="0"/>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>6</v>
+        <v>189</v>
       </c>
       <c r="C506" s="0"/>
       <c r="D506" s="0"/>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B507" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C507" s="0"/>
       <c r="D507" s="0"/>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B508" s="3" t="s">
         <v>29</v>
@@ -8670,30 +8676,30 @@
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>427</v>
+        <v>29</v>
       </c>
       <c r="C509" s="0"/>
       <c r="D509" s="0"/>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>189</v>
+        <v>427</v>
       </c>
       <c r="C510" s="0"/>
       <c r="D510" s="0"/>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>682</v>
+        <v>189</v>
       </c>
       <c r="C511" s="0"/>
       <c r="D511" s="0"/>
@@ -8713,14 +8719,14 @@
         <v>685</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>6</v>
+        <v>686</v>
       </c>
       <c r="C513" s="0"/>
       <c r="D513" s="0"/>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B514" s="3" t="s">
         <v>6</v>
@@ -8730,7 +8736,7 @@
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="2" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B515" s="3" t="s">
         <v>6</v>
@@ -8740,7 +8746,7 @@
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="2" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B516" s="3" t="s">
         <v>6</v>
@@ -8750,7 +8756,7 @@
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B517" s="3" t="s">
         <v>6</v>
@@ -8760,7 +8766,7 @@
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B518" s="3" t="s">
         <v>6</v>
@@ -8770,7 +8776,7 @@
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B519" s="3" t="s">
         <v>6</v>
@@ -8780,7 +8786,7 @@
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="2" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B520" s="3" t="s">
         <v>6</v>
@@ -8790,7 +8796,7 @@
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B521" s="3" t="s">
         <v>6</v>
@@ -8800,7 +8806,7 @@
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B522" s="3" t="s">
         <v>6</v>
@@ -8810,7 +8816,7 @@
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="2" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B523" s="3" t="s">
         <v>6</v>
@@ -8820,47 +8826,47 @@
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="2" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B524" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C524" s="0"/>
       <c r="D524" s="0"/>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B525" s="3" t="s">
-        <v>531</v>
+        <v>29</v>
       </c>
       <c r="C525" s="0"/>
       <c r="D525" s="0"/>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="2" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B526" s="3" t="s">
-        <v>29</v>
+        <v>531</v>
       </c>
       <c r="C526" s="0"/>
       <c r="D526" s="0"/>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B527" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C527" s="0"/>
       <c r="D527" s="0"/>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B528" s="3" t="s">
         <v>6</v>
@@ -8870,47 +8876,47 @@
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="2" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B529" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C529" s="0"/>
       <c r="D529" s="0"/>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B530" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C530" s="0"/>
       <c r="D530" s="0"/>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B531" s="3" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C531" s="0"/>
       <c r="D531" s="0"/>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="2" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B532" s="3" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C532" s="0"/>
       <c r="D532" s="0"/>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="2" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B533" s="3" t="s">
         <v>6</v>
@@ -8920,7 +8926,7 @@
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B534" s="3" t="s">
         <v>6</v>
@@ -8930,7 +8936,7 @@
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B535" s="3" t="s">
         <v>6</v>
@@ -8940,7 +8946,7 @@
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B536" s="3" t="s">
         <v>6</v>
@@ -8950,7 +8956,7 @@
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B537" s="3" t="s">
         <v>6</v>
@@ -8960,7 +8966,7 @@
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B538" s="3" t="s">
         <v>6</v>
@@ -8970,7 +8976,7 @@
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B539" s="3" t="s">
         <v>6</v>
@@ -8980,7 +8986,7 @@
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B540" s="3" t="s">
         <v>6</v>
@@ -8990,7 +8996,7 @@
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B541" s="3" t="s">
         <v>6</v>
@@ -9000,7 +9006,7 @@
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B542" s="3" t="s">
         <v>6</v>
@@ -9010,27 +9016,27 @@
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B543" s="3" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C543" s="0"/>
       <c r="D543" s="0"/>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B544" s="3" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C544" s="0"/>
       <c r="D544" s="0"/>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B545" s="3" t="s">
         <v>6</v>
@@ -9040,7 +9046,7 @@
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B546" s="3" t="s">
         <v>6</v>
@@ -9050,7 +9056,7 @@
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B547" s="3" t="s">
         <v>6</v>
@@ -9060,7 +9066,7 @@
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B548" s="3" t="s">
         <v>6</v>
@@ -9070,7 +9076,7 @@
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B549" s="3" t="s">
         <v>6</v>
@@ -9080,7 +9086,7 @@
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B550" s="3" t="s">
         <v>6</v>
@@ -9090,7 +9096,7 @@
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B551" s="3" t="s">
         <v>6</v>
@@ -9100,7 +9106,7 @@
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B552" s="3" t="s">
         <v>6</v>
@@ -9110,27 +9116,27 @@
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C553" s="0"/>
       <c r="D553" s="0"/>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C554" s="0"/>
       <c r="D554" s="0"/>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B555" s="3" t="s">
         <v>6</v>
@@ -9140,7 +9146,7 @@
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B556" s="3" t="s">
         <v>6</v>
@@ -9150,7 +9156,7 @@
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B557" s="3" t="s">
         <v>6</v>
@@ -9160,7 +9166,7 @@
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B558" s="3" t="s">
         <v>6</v>
@@ -9170,7 +9176,7 @@
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B559" s="3" t="s">
         <v>6</v>
@@ -9180,27 +9186,27 @@
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B560" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C560" s="0"/>
       <c r="D560" s="0"/>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B561" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C561" s="0"/>
       <c r="D561" s="0"/>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B562" s="3" t="s">
         <v>6</v>
@@ -9210,7 +9216,7 @@
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B563" s="3" t="s">
         <v>6</v>
@@ -9220,7 +9226,7 @@
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B564" s="3" t="s">
         <v>6</v>
@@ -9230,7 +9236,7 @@
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B565" s="3" t="s">
         <v>6</v>
@@ -9240,7 +9246,7 @@
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B566" s="3" t="s">
         <v>6</v>
@@ -9250,37 +9256,37 @@
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B567" s="3" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C567" s="0"/>
       <c r="D567" s="0"/>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B568" s="3" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C568" s="0"/>
       <c r="D568" s="0"/>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B569" s="3" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C569" s="0"/>
       <c r="D569" s="0"/>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B570" s="3" t="s">
         <v>6</v>
@@ -9290,7 +9296,7 @@
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B571" s="3" t="s">
         <v>6</v>
@@ -9300,27 +9306,27 @@
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B572" s="3" t="s">
-        <v>469</v>
+        <v>6</v>
       </c>
       <c r="C572" s="0"/>
       <c r="D572" s="0"/>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B573" s="3" t="s">
-        <v>6</v>
+        <v>469</v>
       </c>
       <c r="C573" s="0"/>
       <c r="D573" s="0"/>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B574" s="3" t="s">
         <v>6</v>
@@ -9330,7 +9336,7 @@
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B575" s="3" t="s">
         <v>6</v>
@@ -9340,10 +9346,10 @@
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>749</v>
+        <v>6</v>
       </c>
       <c r="C576" s="0"/>
       <c r="D576" s="0"/>
@@ -9353,14 +9359,14 @@
         <v>750</v>
       </c>
       <c r="B577" s="3" t="s">
-        <v>6</v>
+        <v>751</v>
       </c>
       <c r="C577" s="0"/>
       <c r="D577" s="0"/>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B578" s="3" t="s">
         <v>6</v>
@@ -9370,7 +9376,7 @@
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B579" s="3" t="s">
         <v>6</v>
@@ -9380,7 +9386,7 @@
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B580" s="3" t="s">
         <v>6</v>
@@ -9390,7 +9396,7 @@
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B581" s="3" t="s">
         <v>6</v>
@@ -9400,7 +9406,7 @@
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B582" s="3" t="s">
         <v>6</v>
@@ -9410,7 +9416,7 @@
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B583" s="3" t="s">
         <v>6</v>
@@ -9420,7 +9426,7 @@
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B584" s="3" t="s">
         <v>6</v>
@@ -9430,7 +9436,7 @@
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B585" s="3" t="s">
         <v>6</v>
@@ -9440,7 +9446,7 @@
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B586" s="3" t="s">
         <v>6</v>
@@ -9450,7 +9456,7 @@
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B587" s="3" t="s">
         <v>6</v>
@@ -9460,7 +9466,7 @@
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B588" s="3" t="s">
         <v>6</v>
@@ -9470,7 +9476,7 @@
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B589" s="3" t="s">
         <v>6</v>
@@ -9480,7 +9486,7 @@
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B590" s="3" t="s">
         <v>6</v>
@@ -9490,7 +9496,7 @@
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B591" s="3" t="s">
         <v>6</v>
@@ -9500,7 +9506,7 @@
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B592" s="3" t="s">
         <v>6</v>
@@ -9510,7 +9516,7 @@
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B593" s="3" t="s">
         <v>6</v>
@@ -9520,7 +9526,7 @@
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B594" s="3" t="s">
         <v>6</v>
@@ -9530,7 +9536,7 @@
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B595" s="3" t="s">
         <v>6</v>
@@ -9540,7 +9546,7 @@
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B596" s="3" t="s">
         <v>6</v>
@@ -9550,7 +9556,7 @@
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B597" s="3" t="s">
         <v>6</v>
@@ -9560,7 +9566,7 @@
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B598" s="3" t="s">
         <v>6</v>
@@ -9570,7 +9576,7 @@
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B599" s="3" t="s">
         <v>6</v>
@@ -9580,7 +9586,7 @@
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B600" s="3" t="s">
         <v>6</v>
@@ -9590,7 +9596,7 @@
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B601" s="3" t="s">
         <v>6</v>
@@ -9600,7 +9606,7 @@
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B602" s="3" t="s">
         <v>6</v>
@@ -9610,7 +9616,7 @@
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B603" s="3" t="s">
         <v>6</v>
@@ -9620,7 +9626,7 @@
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B604" s="3" t="s">
         <v>6</v>
@@ -9630,7 +9636,7 @@
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B605" s="3" t="s">
         <v>6</v>
@@ -9640,7 +9646,7 @@
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B606" s="3" t="s">
         <v>6</v>
@@ -9650,7 +9656,7 @@
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B607" s="3" t="s">
         <v>6</v>
@@ -9660,7 +9666,7 @@
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B608" s="3" t="s">
         <v>6</v>
@@ -9670,7 +9676,7 @@
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B609" s="3" t="s">
         <v>6</v>
@@ -9680,7 +9686,7 @@
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B610" s="3" t="s">
         <v>6</v>
@@ -9690,7 +9696,7 @@
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B611" s="3" t="s">
         <v>6</v>
@@ -9700,7 +9706,7 @@
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B612" s="3" t="s">
         <v>6</v>
@@ -9710,7 +9716,7 @@
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B613" s="3" t="s">
         <v>6</v>
@@ -9720,7 +9726,7 @@
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B614" s="3" t="s">
         <v>6</v>
@@ -9730,7 +9736,7 @@
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B615" s="3" t="s">
         <v>6</v>
@@ -9740,7 +9746,7 @@
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B616" s="3" t="s">
         <v>6</v>
@@ -9750,7 +9756,7 @@
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B617" s="3" t="s">
         <v>6</v>
@@ -9760,17 +9766,17 @@
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B618" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C618" s="0"/>
       <c r="D618" s="0"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B619" s="3" t="s">
         <v>29</v>
@@ -9780,17 +9786,17 @@
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B620" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C620" s="0"/>
       <c r="D620" s="0"/>
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B621" s="3" t="s">
         <v>6</v>
@@ -9800,7 +9806,7 @@
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B622" s="3" t="s">
         <v>6</v>
@@ -9810,27 +9816,27 @@
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B623" s="3" t="s">
-        <v>258</v>
+        <v>6</v>
       </c>
       <c r="C623" s="0"/>
       <c r="D623" s="0"/>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B624" s="3" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="C624" s="0"/>
       <c r="D624" s="0"/>
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B625" s="3" t="s">
         <v>6</v>
@@ -9840,27 +9846,27 @@
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B626" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C626" s="0"/>
       <c r="D626" s="0"/>
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B627" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C627" s="0"/>
       <c r="D627" s="0"/>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B628" s="3" t="s">
         <v>6</v>
@@ -9870,7 +9876,7 @@
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B629" s="3" t="s">
         <v>6</v>
@@ -9880,7 +9886,7 @@
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B630" s="3" t="s">
         <v>6</v>
@@ -9890,7 +9896,7 @@
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B631" s="3" t="s">
         <v>6</v>
@@ -9900,7 +9906,7 @@
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B632" s="3" t="s">
         <v>6</v>
@@ -9910,7 +9916,7 @@
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B633" s="3" t="s">
         <v>6</v>
@@ -9920,7 +9926,7 @@
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B634" s="3" t="s">
         <v>6</v>
@@ -9930,7 +9936,7 @@
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B635" s="3" t="s">
         <v>6</v>
@@ -9940,27 +9946,27 @@
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B636" s="3" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C636" s="0"/>
       <c r="D636" s="0"/>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B637" s="3" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C637" s="0"/>
       <c r="D637" s="0"/>
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B638" s="3" t="s">
         <v>6</v>
@@ -9970,7 +9976,7 @@
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B639" s="3" t="s">
         <v>6</v>
@@ -9980,7 +9986,7 @@
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B640" s="3" t="s">
         <v>6</v>
@@ -9990,10 +9996,10 @@
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B641" s="3" t="s">
-        <v>815</v>
+        <v>6</v>
       </c>
       <c r="C641" s="0"/>
       <c r="D641" s="0"/>
@@ -10003,14 +10009,14 @@
         <v>816</v>
       </c>
       <c r="B642" s="3" t="s">
-        <v>6</v>
+        <v>817</v>
       </c>
       <c r="C642" s="0"/>
       <c r="D642" s="0"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B643" s="3" t="s">
         <v>6</v>
@@ -10020,27 +10026,27 @@
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B644" s="3" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C644" s="0"/>
       <c r="D644" s="0"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B645" s="3" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C645" s="0"/>
       <c r="D645" s="0"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B646" s="3" t="s">
         <v>6</v>
@@ -10050,47 +10056,47 @@
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B647" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C647" s="0"/>
       <c r="D647" s="0"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B648" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C648" s="0"/>
       <c r="D648" s="0"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B649" s="3" t="s">
-        <v>258</v>
+        <v>6</v>
       </c>
       <c r="C649" s="0"/>
       <c r="D649" s="0"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B650" s="3" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="C650" s="0"/>
       <c r="D650" s="0"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B651" s="3" t="s">
         <v>6</v>
@@ -10100,7 +10106,7 @@
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B652" s="3" t="s">
         <v>6</v>
@@ -10110,27 +10116,27 @@
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B653" s="3" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="C653" s="0"/>
       <c r="D653" s="0"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B654" s="3" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C654" s="0"/>
       <c r="D654" s="0"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B655" s="3" t="s">
         <v>6</v>
@@ -10140,7 +10146,7 @@
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B656" s="3" t="s">
         <v>6</v>
@@ -10150,7 +10156,7 @@
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B657" s="3" t="s">
         <v>6</v>
@@ -10160,7 +10166,7 @@
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B658" s="3" t="s">
         <v>6</v>
@@ -10170,7 +10176,7 @@
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B659" s="3" t="s">
         <v>6</v>
@@ -10180,27 +10186,27 @@
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B660" s="3" t="s">
-        <v>472</v>
+        <v>6</v>
       </c>
       <c r="C660" s="0"/>
       <c r="D660" s="0"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B661" s="3" t="s">
-        <v>6</v>
+        <v>472</v>
       </c>
       <c r="C661" s="0"/>
       <c r="D661" s="0"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B662" s="3" t="s">
         <v>6</v>
@@ -10210,10 +10216,10 @@
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B663" s="3" t="s">
-        <v>838</v>
+        <v>6</v>
       </c>
       <c r="C663" s="0"/>
       <c r="D663" s="0"/>
@@ -10223,24 +10229,24 @@
         <v>839</v>
       </c>
       <c r="B664" s="3" t="s">
-        <v>569</v>
+        <v>840</v>
       </c>
       <c r="C664" s="0"/>
       <c r="D664" s="0"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B665" s="3" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="C665" s="0"/>
       <c r="D665" s="0"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B666" s="3" t="s">
         <v>6</v>
@@ -10250,7 +10256,7 @@
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B667" s="3" t="s">
         <v>6</v>
@@ -10260,7 +10266,7 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B668" s="3" t="s">
         <v>6</v>
@@ -10270,17 +10276,17 @@
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B669" s="3" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C669" s="0"/>
       <c r="D669" s="0"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B670" s="3" t="s">
         <v>63</v>
@@ -10290,17 +10296,17 @@
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B671" s="3" t="s">
-        <v>569</v>
+        <v>63</v>
       </c>
       <c r="C671" s="0"/>
       <c r="D671" s="0"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B672" s="3" t="s">
         <v>569</v>
@@ -10310,17 +10316,17 @@
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B673" s="3" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="C673" s="0"/>
       <c r="D673" s="0"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B674" s="3" t="s">
         <v>6</v>
@@ -10330,30 +10336,30 @@
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B675" s="3" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C675" s="0"/>
       <c r="D675" s="0"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B676" s="3" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C676" s="0"/>
       <c r="D676" s="0"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B677" s="3" t="s">
-        <v>853</v>
+        <v>6</v>
       </c>
       <c r="C677" s="0"/>
       <c r="D677" s="0"/>
@@ -10363,24 +10369,24 @@
         <v>854</v>
       </c>
       <c r="B678" s="3" t="s">
-        <v>29</v>
+        <v>855</v>
       </c>
       <c r="C678" s="0"/>
       <c r="D678" s="0"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B679" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C679" s="0"/>
       <c r="D679" s="0"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B680" s="3" t="s">
         <v>6</v>
@@ -10390,7 +10396,7 @@
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B681" s="3" t="s">
         <v>6</v>
@@ -10400,7 +10406,7 @@
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B682" s="3" t="s">
         <v>6</v>
@@ -10410,7 +10416,7 @@
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B683" s="3" t="s">
         <v>6</v>
@@ -10420,7 +10426,7 @@
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B684" s="3" t="s">
         <v>6</v>
@@ -10430,7 +10436,7 @@
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B685" s="3" t="s">
         <v>6</v>
@@ -10440,7 +10446,7 @@
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B686" s="3" t="s">
         <v>6</v>
@@ -10450,7 +10456,7 @@
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B687" s="3" t="s">
         <v>6</v>
@@ -10460,7 +10466,7 @@
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B688" s="3" t="s">
         <v>6</v>
@@ -10470,7 +10476,7 @@
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B689" s="3" t="s">
         <v>6</v>
@@ -10480,10 +10486,10 @@
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B690" s="3" t="s">
-        <v>867</v>
+        <v>6</v>
       </c>
       <c r="C690" s="0"/>
       <c r="D690" s="0"/>
@@ -10493,24 +10499,24 @@
         <v>868</v>
       </c>
       <c r="B691" s="3" t="s">
-        <v>112</v>
+        <v>869</v>
       </c>
       <c r="C691" s="0"/>
       <c r="D691" s="0"/>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B692" s="3" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C692" s="0"/>
       <c r="D692" s="0"/>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B693" s="3" t="s">
         <v>6</v>
@@ -10520,7 +10526,7 @@
     </row>
     <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B694" s="3" t="s">
         <v>6</v>
@@ -10530,47 +10536,47 @@
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B695" s="3" t="s">
-        <v>815</v>
+        <v>6</v>
       </c>
       <c r="C695" s="0"/>
       <c r="D695" s="0"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B696" s="3" t="s">
-        <v>6</v>
+        <v>817</v>
       </c>
       <c r="C696" s="0"/>
       <c r="D696" s="0"/>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B697" s="3" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C697" s="0"/>
       <c r="D697" s="0"/>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B698" s="3" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C698" s="0"/>
       <c r="D698" s="0"/>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B699" s="3" t="s">
         <v>6</v>
@@ -10580,27 +10586,27 @@
     </row>
     <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B700" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C700" s="0"/>
       <c r="D700" s="0"/>
     </row>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B701" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C701" s="0"/>
       <c r="D701" s="0"/>
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B702" s="3" t="s">
         <v>6</v>
@@ -10610,7 +10616,7 @@
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B703" s="3" t="s">
         <v>6</v>
@@ -10620,7 +10626,7 @@
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B704" s="3" t="s">
         <v>6</v>
@@ -10630,7 +10636,7 @@
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B705" s="3" t="s">
         <v>6</v>
@@ -10640,7 +10646,7 @@
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B706" s="3" t="s">
         <v>6</v>
@@ -10650,7 +10656,7 @@
     </row>
     <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B707" s="3" t="s">
         <v>6</v>
@@ -10660,47 +10666,47 @@
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B708" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C708" s="0"/>
       <c r="D708" s="0"/>
     </row>
     <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B709" s="3" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="C709" s="0"/>
       <c r="D709" s="0"/>
     </row>
     <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B710" s="3" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="C710" s="0"/>
       <c r="D710" s="0"/>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B711" s="3" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="C711" s="0"/>
       <c r="D711" s="0"/>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B712" s="3" t="s">
         <v>6</v>
@@ -10710,7 +10716,7 @@
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B713" s="3" t="s">
         <v>6</v>
@@ -10720,7 +10726,7 @@
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B714" s="3" t="s">
         <v>6</v>
@@ -10730,7 +10736,7 @@
     </row>
     <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B715" s="3" t="s">
         <v>6</v>
@@ -10740,7 +10746,7 @@
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B716" s="3" t="s">
         <v>6</v>
@@ -10750,14 +10756,25 @@
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B717" s="3" t="s">
-        <v>472</v>
+        <v>6</v>
       </c>
       <c r="C717" s="0"/>
       <c r="D717" s="0"/>
     </row>
+    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B718" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C718" s="0"/>
+      <c r="D718" s="0"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -10776,8 +10793,8 @@
   </sheetPr>
   <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10803,7 +10820,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -10818,7 +10835,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>29</v>
@@ -10828,7 +10845,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>29</v>
@@ -10838,7 +10855,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -10848,7 +10865,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>6</v>
@@ -10858,7 +10875,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
@@ -10868,17 +10885,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>63</v>
@@ -10888,7 +10905,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>6</v>
@@ -10898,7 +10915,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>10</v>
@@ -10908,7 +10925,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>10</v>
@@ -10918,27 +10935,27 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>293</v>
@@ -10948,7 +10965,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>10</v>
@@ -10978,7 +10995,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>10</v>
@@ -10988,7 +11005,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>10</v>
@@ -11081,7 +11098,7 @@
         <v>183</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="C30" s="0"/>
       <c r="D30" s="0"/>
@@ -11091,14 +11108,14 @@
         <v>199</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>10</v>
@@ -11108,20 +11125,20 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="C34" s="0"/>
       <c r="D34" s="0"/>
@@ -11168,127 +11185,127 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="C39" s="0"/>
       <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C40" s="0"/>
       <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C41" s="0"/>
       <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C43" s="0"/>
       <c r="D43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C44" s="0"/>
       <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="C45" s="0"/>
       <c r="D45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="C46" s="0"/>
       <c r="D46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C47" s="0"/>
       <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="C48" s="0"/>
       <c r="D48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C49" s="0"/>
       <c r="D49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C50" s="0"/>
       <c r="D50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>107</v>
@@ -11298,7 +11315,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>125</v>
@@ -11308,47 +11325,47 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C53" s="0"/>
       <c r="D53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C54" s="0"/>
       <c r="D54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="C55" s="0"/>
       <c r="D55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C56" s="0"/>
       <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>6</v>
@@ -11358,7 +11375,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>29</v>
@@ -11368,7 +11385,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>19</v>
@@ -11378,7 +11395,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>10</v>
@@ -11388,7 +11405,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>10</v>
@@ -11398,7 +11415,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>10</v>
@@ -11408,77 +11425,77 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C63" s="0"/>
       <c r="D63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C64" s="0"/>
       <c r="D64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C65" s="0"/>
       <c r="D65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C66" s="0"/>
       <c r="D66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C67" s="0"/>
       <c r="D67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C68" s="0"/>
       <c r="D68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="C69" s="0"/>
       <c r="D69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>100</v>
@@ -11488,47 +11505,47 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C72" s="0"/>
       <c r="D72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="C73" s="0"/>
       <c r="D73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>107</v>
@@ -11538,7 +11555,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>125</v>
@@ -11548,47 +11565,47 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C77" s="0"/>
       <c r="D77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C80" s="0"/>
       <c r="D80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>6</v>
@@ -11598,7 +11615,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>29</v>
@@ -11608,7 +11625,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>19</v>
@@ -11618,17 +11635,17 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C84" s="0"/>
       <c r="D84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>10</v>
@@ -11638,7 +11655,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>10</v>
@@ -11651,14 +11668,14 @@
         <v>254</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C87" s="0"/>
       <c r="D87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>10</v>
@@ -11668,7 +11685,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>10</v>
@@ -11678,7 +11695,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>10</v>
@@ -11688,7 +11705,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>10</v>
@@ -11698,7 +11715,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>115</v>
@@ -11708,7 +11725,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>115</v>
@@ -11718,7 +11735,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>6</v>
@@ -11728,7 +11745,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>6</v>
@@ -11738,40 +11755,40 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C96" s="0"/>
       <c r="D96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C97" s="0"/>
       <c r="D97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B99" s="0" t="s">
         <v>1002</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>1000</v>
       </c>
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
@@ -11811,14 +11828,14 @@
         <v>524</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="C103" s="0"/>
       <c r="D103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>10</v>
@@ -11828,7 +11845,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>10</v>
@@ -11838,7 +11855,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>10</v>
@@ -11848,7 +11865,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>10</v>
@@ -11858,7 +11875,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>10</v>
@@ -11868,17 +11885,17 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C109" s="0"/>
       <c r="D109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>10</v>
@@ -11888,7 +11905,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>29</v>
@@ -11898,7 +11915,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>29</v>
@@ -11908,7 +11925,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>29</v>
@@ -11918,7 +11935,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>29</v>
@@ -11928,17 +11945,17 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>63</v>
@@ -11948,7 +11965,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>6</v>
@@ -11958,7 +11975,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>63</v>
@@ -11968,7 +11985,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>6</v>
@@ -11978,7 +11995,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>6</v>
@@ -11988,7 +12005,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>6</v>
@@ -11998,7 +12015,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>6</v>
@@ -12008,7 +12025,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>6</v>
@@ -12018,7 +12035,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>6</v>
@@ -12028,7 +12045,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>6</v>
@@ -12038,7 +12055,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>6</v>
@@ -12048,7 +12065,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>6</v>
@@ -12058,7 +12075,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>6</v>
@@ -12068,7 +12085,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>6</v>
@@ -12078,7 +12095,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>6</v>
@@ -12088,7 +12105,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>6</v>
@@ -12098,7 +12115,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>6</v>
@@ -12108,7 +12125,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>6</v>
@@ -12118,7 +12135,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>112</v>
@@ -12128,7 +12145,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>112</v>
@@ -12138,7 +12155,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>569</v>
@@ -12148,7 +12165,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>569</v>
@@ -12158,7 +12175,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>6</v>
@@ -12168,7 +12185,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B139" s="0" t="s">
         <v>6</v>
@@ -12178,7 +12195,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>569</v>
@@ -12188,7 +12205,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B141" s="0" t="s">
         <v>6</v>
@@ -12198,7 +12215,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>29</v>
@@ -12208,7 +12225,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B143" s="0" t="s">
         <v>6</v>
@@ -12218,7 +12235,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="B144" s="0" t="s">
         <v>531</v>
@@ -12228,7 +12245,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>6</v>
@@ -12238,7 +12255,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>6</v>
@@ -12248,7 +12265,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>569</v>
@@ -12258,7 +12275,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B148" s="0" t="s">
         <v>6</v>
@@ -12268,7 +12285,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B149" s="0" t="s">
         <v>6</v>
@@ -12278,7 +12295,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B150" s="0" t="s">
         <v>29</v>
@@ -12288,7 +12305,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>531</v>
@@ -12298,7 +12315,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="B152" s="0" t="s">
         <v>29</v>
@@ -12308,7 +12325,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B153" s="0" t="s">
         <v>569</v>
@@ -12318,7 +12335,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="B154" s="0" t="s">
         <v>134</v>
@@ -12328,7 +12345,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B155" s="0" t="s">
         <v>134</v>
@@ -12338,7 +12355,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="B156" s="0" t="s">
         <v>569</v>
@@ -12348,7 +12365,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="B157" s="0" t="s">
         <v>29</v>
@@ -12358,17 +12375,17 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C158" s="0"/>
       <c r="D158" s="0"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="B159" s="0" t="s">
         <v>6</v>
@@ -12378,7 +12395,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B160" s="0" t="s">
         <v>6</v>
@@ -12388,7 +12405,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>115</v>
@@ -12398,17 +12415,17 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="C162" s="0"/>
       <c r="D162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="B163" s="0" t="s">
         <v>6</v>
@@ -12418,7 +12435,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>6</v>
@@ -12428,7 +12445,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B165" s="0" t="s">
         <v>115</v>
@@ -12438,7 +12455,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>6</v>
@@ -12448,7 +12465,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="B167" s="0" t="s">
         <v>63</v>
@@ -12458,7 +12475,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B168" s="0" t="s">
         <v>6</v>
@@ -12468,7 +12485,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>6</v>
@@ -12478,7 +12495,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B170" s="0" t="s">
         <v>115</v>
@@ -12488,7 +12505,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>115</v>
@@ -12498,7 +12515,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>6</v>
@@ -12508,7 +12525,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="B173" s="0" t="s">
         <v>6</v>
@@ -12518,7 +12535,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="B174" s="0" t="s">
         <v>6</v>
@@ -12528,7 +12545,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="B175" s="0" t="s">
         <v>6</v>
@@ -12538,7 +12555,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="B176" s="0" t="s">
         <v>6</v>
@@ -12548,7 +12565,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B177" s="0" t="s">
         <v>265</v>
@@ -12558,7 +12575,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B178" s="0" t="s">
         <v>6</v>
@@ -12568,7 +12585,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B179" s="0" t="s">
         <v>6</v>
@@ -12578,7 +12595,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>6</v>
@@ -12588,7 +12605,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>6</v>
@@ -12615,7 +12632,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E:E A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12637,7 +12654,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12650,18 +12667,18 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2.55</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2.55</v>
@@ -12686,7 +12703,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="E:E C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12698,78 +12715,78 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="4" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="4" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12777,31 +12794,31 @@
         <v>428</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="6" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="6" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="6" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12809,7 +12826,7 @@
         <v>444</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12817,25 +12834,25 @@
         <v>445</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="6" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="6" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -12843,7 +12860,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="6" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
@@ -12851,7 +12868,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1</v>
@@ -12871,146 +12888,146 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="4" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>